<commit_message>
Testing save function: not working yet. Find function: yes.
</commit_message>
<xml_diff>
--- a/voluntariatApp/voluntariatApp/Baza de date.xlsx
+++ b/voluntariatApp/voluntariatApp/Baza de date.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\info\ProiectTechTrek\voluntariatApp\voluntariatApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8178D285-45B0-4299-9703-580B1742C260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-21528" yWindow="1020" windowWidth="21624" windowHeight="11244" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Logins" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Eveniment" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Inscriere" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Participare" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Organizator" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="User" sheetId="6" r:id="rId9"/>
+    <sheet name="Logins" sheetId="1" r:id="rId1"/>
+    <sheet name="Eveniment" sheetId="2" r:id="rId2"/>
+    <sheet name="Inscriere" sheetId="3" r:id="rId3"/>
+    <sheet name="Participare" sheetId="4" r:id="rId4"/>
+    <sheet name="Organizator" sheetId="5" r:id="rId5"/>
+    <sheet name="User" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="113">
   <si>
     <t>id(string)</t>
   </si>
@@ -340,44 +349,71 @@
   </si>
   <si>
     <t>Maria Vladislav</t>
+  </si>
+  <si>
+    <t>5020505125000</t>
+  </si>
+  <si>
+    <t>50205051251230</t>
+  </si>
+  <si>
+    <t>5020505125325</t>
+  </si>
+  <si>
+    <t>5020505125324</t>
+  </si>
+  <si>
+    <t>5020505125678</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm-dd-yyyy h:mm"/>
+    <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy\ h:mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -385,7 +421,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -401,79 +437,58 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -663,23 +678,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="23.13"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,92 +714,92 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>5.020505125E12</v>
+        <v>5020505125000</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>1234.0</v>
+        <v>1234</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="3">
-        <v>7.33333331E8</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>733333331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>5.020505125123E13</v>
+        <v>50205051251230</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>1234.0</v>
+        <v>1234</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="4">
-        <v>7.33333431E8</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>733333431</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>5.020505125325E12</v>
+        <v>5020505125325</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>1234.0</v>
+        <v>1234</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="3">
-        <v>7.33365331E8</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>733365331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>5.020505125324E12</v>
+        <v>5020505125324</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2">
-        <v>1234.0</v>
+        <v>1234</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="3">
-        <v>7.32433331E8</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>732433331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>5.020505125678E12</v>
+        <v>5020505125678</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2">
-        <v>1234.0</v>
+        <v>1234</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="3">
-        <v>7.33421351E8</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>733421351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -789,16 +807,16 @@
         <v>16</v>
       </c>
       <c r="C7" s="2">
-        <v>1234.0</v>
+        <v>1234</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="3">
-        <v>7.33333331E8</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>733333331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
@@ -806,41 +824,42 @@
         <v>19</v>
       </c>
       <c r="C8" s="2">
-        <v>1234.0</v>
+        <v>1234</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="3">
-        <v>7.33333331E8</v>
+        <v>733333331</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.38"/>
-    <col customWidth="1" min="2" max="2" width="18.13"/>
-    <col customWidth="1" min="3" max="3" width="36.0"/>
-    <col customWidth="1" min="4" max="4" width="12.25"/>
-    <col customWidth="1" min="6" max="6" width="26.75"/>
-    <col customWidth="1" min="7" max="7" width="32.88"/>
-    <col customWidth="1" min="8" max="8" width="41.25"/>
-    <col customWidth="1" min="9" max="9" width="80.38"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" customWidth="1"/>
+    <col min="9" max="9" width="80.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -869,9 +888,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>18</v>
@@ -880,7 +899,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>31</v>
@@ -898,9 +917,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>18</v>
@@ -909,7 +928,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="2">
-        <v>500.0</v>
+        <v>500</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>35</v>
@@ -927,9 +946,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>18</v>
@@ -938,7 +957,7 @@
         <v>37</v>
       </c>
       <c r="D4" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>38</v>
@@ -956,9 +975,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>15</v>
@@ -967,7 +986,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>38</v>
@@ -985,9 +1004,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
@@ -996,7 +1015,7 @@
         <v>42</v>
       </c>
       <c r="D6" s="2">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>35</v>
@@ -1014,20 +1033,20 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="7">
-        <v>40.0</v>
-      </c>
-      <c r="E7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F7" s="6">
@@ -1039,26 +1058,26 @@
       <c r="H7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8">
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
-        <v>8.3475993E7</v>
-      </c>
-      <c r="C8" s="8" t="s">
+        <v>83475993</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D8" s="7">
-        <v>20.0</v>
-      </c>
-      <c r="E8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="6">
@@ -1070,26 +1089,26 @@
       <c r="H8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5">
-        <v>8.3475993E7</v>
-      </c>
-      <c r="C9" s="8" t="s">
+        <v>83475993</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="7">
-        <v>100.0</v>
-      </c>
-      <c r="E9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>52</v>
       </c>
       <c r="F9" s="6">
@@ -1101,26 +1120,26 @@
       <c r="H9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10">
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5">
-        <v>8.3475993E7</v>
-      </c>
-      <c r="C10" s="8" t="s">
+        <v>83475993</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="7">
-        <v>300.0</v>
-      </c>
-      <c r="E10" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>55</v>
       </c>
       <c r="F10" s="6">
@@ -1132,26 +1151,26 @@
       <c r="H10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11">
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5">
-        <v>8.3475993E7</v>
-      </c>
-      <c r="C11" s="8" t="s">
+        <v>83475993</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>57</v>
       </c>
       <c r="D11" s="7">
-        <v>15.0</v>
-      </c>
-      <c r="E11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>52</v>
       </c>
       <c r="F11" s="6">
@@ -1163,15 +1182,15 @@
       <c r="H11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12">
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>59</v>
@@ -1180,7 +1199,7 @@
         <v>60</v>
       </c>
       <c r="D12" s="2">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>61</v>
@@ -1188,7 +1207,7 @@
       <c r="F12" s="6">
         <v>45357.5</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>62</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1198,9 +1217,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>59</v>
@@ -1209,7 +1228,7 @@
         <v>65</v>
       </c>
       <c r="D13" s="2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>66</v>
@@ -1227,9 +1246,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>59</v>
@@ -1238,7 +1257,7 @@
         <v>69</v>
       </c>
       <c r="D14" s="2">
-        <v>250.0</v>
+        <v>250</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>52</v>
@@ -1256,9 +1275,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>59</v>
@@ -1267,7 +1286,7 @@
         <v>72</v>
       </c>
       <c r="D15" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>52</v>
@@ -1275,7 +1294,7 @@
       <c r="F15" s="6">
         <v>45297.416666666664</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="8" t="s">
         <v>73</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -1286,25 +1305,26 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="27.75"/>
-    <col customWidth="1" min="4" max="4" width="34.0"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -1321,12 +1341,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>5.020505125E12</v>
+        <v>5020505125000</v>
       </c>
       <c r="B2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="6">
         <v>45328.5</v>
@@ -1338,12 +1358,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>5.020505125123E13</v>
+        <v>50205051251230</v>
       </c>
       <c r="B3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="6">
         <v>45328.5</v>
@@ -1355,12 +1375,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>5.020505125325E12</v>
+        <v>5020505125325</v>
       </c>
       <c r="B4" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="6">
         <v>45328.5</v>
@@ -1372,12 +1392,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>5.020505125E12</v>
+        <v>5020505125000</v>
       </c>
       <c r="B5" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="6">
         <v>45328.5</v>
@@ -1389,12 +1409,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>5.020505125678E12</v>
+        <v>5020505125678</v>
       </c>
       <c r="B6" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6">
         <v>45328.5</v>
@@ -1406,12 +1426,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>5.020505125678E12</v>
+        <v>5020505125678</v>
       </c>
       <c r="B7" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C7" s="6">
         <v>45328.5</v>
@@ -1423,12 +1443,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>5.020505125324E12</v>
+        <v>5020505125324</v>
       </c>
       <c r="B8" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="6">
         <v>45328.5</v>
@@ -1440,12 +1460,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>5.020505125324E12</v>
+        <v>5020505125324</v>
       </c>
       <c r="B9" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C9" s="6">
         <v>45328.5</v>
@@ -1458,24 +1478,25 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="31.25"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>76</v>
       </c>
@@ -1488,14 +1509,14 @@
       <c r="D1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="10"/>
-    </row>
-    <row r="2">
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>5.020505125E12</v>
+        <v>5020505125000</v>
       </c>
       <c r="B2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -1504,12 +1525,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>5.020505125123E13</v>
+        <v>50205051251230</v>
       </c>
       <c r="B3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -1518,12 +1539,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>5.020505125325E12</v>
+        <v>5020505125325</v>
       </c>
       <c r="B4" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -1532,12 +1553,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>5.020505125E12</v>
+        <v>5020505125000</v>
       </c>
       <c r="B5" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>0</v>
@@ -1546,12 +1567,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>5.020505125678E12</v>
+        <v>5020505125678</v>
       </c>
       <c r="B6" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -1560,12 +1581,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>5.020505125678E12</v>
+        <v>5020505125678</v>
       </c>
       <c r="B7" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -1574,12 +1595,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>5.020505125324E12</v>
+        <v>5020505125324</v>
       </c>
       <c r="B8" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>1</v>
@@ -1588,12 +1609,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>5.020505125324E12</v>
+        <v>5020505125324</v>
       </c>
       <c r="B9" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>1</v>
@@ -1603,26 +1624,27 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.75"/>
-    <col customWidth="1" min="2" max="2" width="25.63"/>
-    <col customWidth="1" min="4" max="4" width="58.25"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="58.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1636,7 +1658,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>59</v>
       </c>
@@ -1650,9 +1672,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>8.3475993E7</v>
+        <v>83475993</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>92</v>
@@ -1664,7 +1686,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1678,7 +1700,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1693,22 +1715,28 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" style="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1721,77 +1749,77 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>5.020505125E12</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>99</v>
       </c>
       <c r="C2" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2">
-        <v>5.020505125123E13</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>109</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>101</v>
       </c>
       <c r="C3" s="2">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2">
-        <v>5.020505125325E12</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>103</v>
       </c>
       <c r="C4" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>5.020505125324E12</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>105</v>
       </c>
       <c r="C5" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2">
-        <v>5.020505125678E12</v>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>107</v>
       </c>
       <c r="C6" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>